<commit_message>
updates with 2023 data
</commit_message>
<xml_diff>
--- a/plots/Figure 3.xlsx
+++ b/plots/Figure 3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\SESAM\EP-LikeMindedness\plots\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorenzorinaldi/Documents/GitHub/SESAM/GeoP_LikeMindedness_EU-gas/plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85849F0E-7987-450E-8791-823923BD1174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325C874C-DD3E-9341-B5B1-DC2854758DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{4E1F33B5-9651-4FAD-A3EA-AF1CA21127EE}"/>
+    <workbookView xWindow="-9240" yWindow="-28300" windowWidth="51200" windowHeight="27020" xr2:uid="{4E1F33B5-9651-4FAD-A3EA-AF1CA21127EE}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="19">
   <si>
     <t>Hybrid</t>
   </si>
@@ -80,18 +80,6 @@
     <t>AZE</t>
   </si>
   <si>
-    <t>Pure Liberal</t>
-  </si>
-  <si>
-    <t>Pure Realistic</t>
-  </si>
-  <si>
-    <t>Liberal</t>
-  </si>
-  <si>
-    <t>Realistic</t>
-  </si>
-  <si>
     <t>Pipeline import</t>
   </si>
   <si>
@@ -99,6 +87,12 @@
   </si>
   <si>
     <t>Weighted avg LMI</t>
+  </si>
+  <si>
+    <t>Normative</t>
+  </si>
+  <si>
+    <t>Pragmatic</t>
   </si>
 </sst>
 </file>
@@ -186,8 +180,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Percentuale" xfId="1" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -219,7 +213,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="it-IT"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -268,10 +262,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Liberal</c:v>
+                  <c:v>Normative</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Realistic</c:v>
+                  <c:v>Pragmatic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Hybrid</c:v>
@@ -333,10 +327,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Liberal</c:v>
+                  <c:v>Normative</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Realistic</c:v>
+                  <c:v>Pragmatic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Hybrid</c:v>
@@ -399,10 +393,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Liberal</c:v>
+                  <c:v>Normative</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Realistic</c:v>
+                  <c:v>Pragmatic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Hybrid</c:v>
@@ -465,10 +459,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Liberal</c:v>
+                  <c:v>Normative</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Realistic</c:v>
+                  <c:v>Pragmatic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Hybrid</c:v>
@@ -530,10 +524,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Liberal</c:v>
+                  <c:v>Normative</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Realistic</c:v>
+                  <c:v>Pragmatic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Hybrid</c:v>
@@ -595,10 +589,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Liberal</c:v>
+                  <c:v>Normative</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Realistic</c:v>
+                  <c:v>Pragmatic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Hybrid</c:v>
@@ -660,10 +654,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Liberal</c:v>
+                  <c:v>Normative</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Realistic</c:v>
+                  <c:v>Pragmatic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Hybrid</c:v>
@@ -726,10 +720,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Liberal</c:v>
+                  <c:v>Normative</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Realistic</c:v>
+                  <c:v>Pragmatic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Hybrid</c:v>
@@ -791,10 +785,10 @@
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Liberal</c:v>
+                  <c:v>Normative</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Realistic</c:v>
+                  <c:v>Pragmatic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Hybrid</c:v>
@@ -1243,7 +1237,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="it-IT"/>
+                <a:endParaRPr lang="en-IT"/>
               </a:p>
             </c:txPr>
             <c:showLegendKey val="0"/>
@@ -1280,13 +1274,13 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.2100005557305318E-2</c:v>
+                  <c:v>4.4613546354331464E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.19327446053265279</c:v>
+                  <c:v>-0.1811508540537842</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.13905147664442982</c:v>
+                  <c:v>-0.12762720048254272</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1363,7 +1357,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1791884016"/>
@@ -1437,7 +1431,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="it-IT"/>
+              <a:endParaRPr lang="en-IT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1466,7 +1460,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1789453312"/>
@@ -1517,7 +1511,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="it-IT"/>
+              <a:endParaRPr lang="en-IT"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1546,7 +1540,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="it-IT"/>
+            <a:endParaRPr lang="en-IT"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="349596960"/>
@@ -1625,7 +1619,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="it-IT"/>
+          <a:endParaRPr lang="en-IT"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1664,7 +1658,7 @@
           <a:latin typeface="HelveticaNeue Light" panose="00000400000000000000" pitchFamily="2" charset="0"/>
         </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="it-IT"/>
+      <a:endParaRPr lang="en-IT"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2317,9 +2311,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2357,7 +2351,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2463,7 +2457,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2605,7 +2599,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2615,30 +2609,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EED9DF-830F-4EDC-A3CF-E2C04646B67A}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="4" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="4" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B1" s="8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5" t="s">
         <v>1</v>
@@ -2661,12 +2655,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>0.114575867676486</v>
+        <v>0.12667244233304609</v>
       </c>
       <c r="C3" s="2">
         <v>0.13774523259164501</v>
@@ -2677,7 +2671,7 @@
         <v>3</v>
       </c>
       <c r="G3" s="1">
-        <v>0.114575867676486</v>
+        <v>0.12667244233304609</v>
       </c>
       <c r="H3" s="2">
         <v>0.13774523259164501</v>
@@ -2686,18 +2680,18 @@
         <v>3</v>
       </c>
       <c r="L3" s="1">
-        <v>0.114575867676486</v>
+        <v>0.12667244233304609</v>
       </c>
       <c r="M3" s="2">
         <v>0.13774523259164501</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <v>4.5112294870626797E-2</v>
+        <v>3.3909185897802341E-2</v>
       </c>
       <c r="C4" s="2">
         <v>0.82591572602923302</v>
@@ -2708,7 +2702,7 @@
         <v>5</v>
       </c>
       <c r="G4" s="1">
-        <v>-0.33820652098381399</v>
+        <v>-0.32050758414456437</v>
       </c>
       <c r="H4" s="2">
         <v>0.21912853882268299</v>
@@ -2717,18 +2711,18 @@
         <v>6</v>
       </c>
       <c r="L4" s="1">
-        <v>-0.25337528973048301</v>
+        <v>-0.27645523201180838</v>
       </c>
       <c r="M4" s="2">
         <v>7.0238091615336201E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="6">
-        <v>-2.5901281937534298E-2</v>
+        <v>-2.3146140781594826E-2</v>
       </c>
       <c r="C5" s="7">
         <f>1-SUM(C3:C4)</f>
@@ -2740,7 +2734,7 @@
         <v>8</v>
       </c>
       <c r="G5" s="1">
-        <v>-0.40194801835590899</v>
+        <v>-0.40269935060031564</v>
       </c>
       <c r="H5" s="2">
         <v>5.3818284092682599E-2</v>
@@ -2749,25 +2743,25 @@
         <v>9</v>
       </c>
       <c r="L5" s="1">
-        <v>-0.26357623393471002</v>
+        <v>-0.22674358641384296</v>
       </c>
       <c r="M5" s="2">
         <v>0.18443952258603499</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4">
         <f>SUMPRODUCT(B3:B5,C3:C5)</f>
-        <v>5.2100005557305318E-2</v>
+        <v>4.4613546354331464E-2</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="1">
-        <v>-0.39183983751845902</v>
+        <v>-0.38405830709612232</v>
       </c>
       <c r="H6" s="2">
         <v>0.10448765234304599</v>
@@ -2776,25 +2770,25 @@
         <v>5</v>
       </c>
       <c r="L6" s="1">
-        <v>-0.33820652098381399</v>
+        <v>-0.32050758414456437</v>
       </c>
       <c r="M6" s="2">
         <v>0.21912853882268299</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4">
         <f>AVERAGE(B3:B5)</f>
-        <v>4.4595626869859496E-2</v>
+        <v>4.5811829149751203E-2</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="G7" s="1">
-        <v>-0.26357623393471002</v>
+        <v>-0.22674358641384296</v>
       </c>
       <c r="H7" s="2">
         <v>0.18443952258603499</v>
@@ -2803,18 +2797,18 @@
         <v>13</v>
       </c>
       <c r="L7" s="1">
-        <v>-0.36778278499450301</v>
+        <v>-0.39420734792308348</v>
       </c>
       <c r="M7" s="2">
         <v>1.2434913093894299E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F8" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="1">
-        <v>-0.25337528973048301</v>
+        <v>-0.27645523201180838</v>
       </c>
       <c r="H8" s="2">
         <v>7.0238091615336201E-2</v>
@@ -2823,19 +2817,19 @@
         <v>7</v>
       </c>
       <c r="L8" s="6">
-        <v>-2.5901281937534298E-2</v>
+        <v>-2.3146140781594826E-2</v>
       </c>
       <c r="M8" s="7">
         <f>1-SUM(M3:M7)</f>
         <v>0.37601370129040645</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="6">
-        <v>-2.5901281937534298E-2</v>
+        <v>-2.3146140781594826E-2</v>
       </c>
       <c r="H9" s="7">
         <f>1-SUM(H3:H8)</f>
@@ -2846,46 +2840,46 @@
       </c>
       <c r="L9" s="4">
         <f>SUMPRODUCT(L3:L8,M3:M8)</f>
-        <v>-0.13905147664442982</v>
+        <v>-0.12762720048254272</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F10" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G10" s="4">
         <f>SUMPRODUCT(G3:G9,H3:H9)</f>
-        <v>-0.19327446053265279</v>
+        <v>-0.1811508540537842</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="L10" s="4">
         <f>AVERAGE(L3:L8)</f>
-        <v>-0.1890443739840931</v>
+        <v>-0.18573124149030798</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="F11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="4">
         <f>AVERAGE(G3:G9)</f>
-        <v>-0.22289590211206051</v>
+        <v>-0.21527682267360035</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -2902,7 +2896,7 @@
         <v>0.13774523259164501</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -2919,7 +2913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -2936,7 +2930,7 @@
         <v>0.37601370129040645</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -2953,7 +2947,7 @@
         <v>0.21912853882268299</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2970,7 +2964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -2987,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -3004,7 +2998,7 @@
         <v>0.18443952258603499</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -3021,7 +3015,7 @@
         <v>7.0238091615336201E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -3038,67 +3032,67 @@
         <v>1.2434913093894299E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B33" s="2">
         <f>B6</f>
-        <v>5.2100005557305318E-2</v>
+        <v>4.4613546354331464E-2</v>
       </c>
       <c r="C33" s="2">
         <f>G10</f>
-        <v>-0.19327446053265279</v>
+        <v>-0.1811508540537842</v>
       </c>
       <c r="D33" s="2">
         <f>L9</f>
-        <v>-0.13905147664442982</v>
+        <v>-0.12762720048254272</v>
       </c>
     </row>
   </sheetData>
@@ -3109,6 +3103,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e67e9a88-35e1-4b39-8da9-a609eb308282" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100241E96938535DD4B921FCDFB54345D30" ma:contentTypeVersion="17" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="24b4a5ee6c90ad5e302ffe9a945ebb1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e" xmlns:ns3="e67e9a88-35e1-4b39-8da9-a609eb308282" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0be869e1b59aa26d60130e74dad6d347" ns2:_="" ns3:_="">
     <xsd:import namespace="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
@@ -3357,27 +3371,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F84659C0-8E19-4071-B782-A53C79575036}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
+    <ds:schemaRef ds:uri="e67e9a88-35e1-4b39-8da9-a609eb308282"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e67e9a88-35e1-4b39-8da9-a609eb308282" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E0654D-932E-40AB-B5E8-4C66F2667012}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64BC88C7-C7F4-43C9-AB6F-B25AF2705778}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3394,23 +3407,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6E0654D-932E-40AB-B5E8-4C66F2667012}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F84659C0-8E19-4071-B782-A53C79575036}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5d44ae6a-e145-4c9d-94e7-ddf9cc58067e"/>
-    <ds:schemaRef ds:uri="e67e9a88-35e1-4b39-8da9-a609eb308282"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>